<commit_message>
Load data from XML
https://github.com/Team-Roc/WeaponsFactory/issues/5
</commit_message>
<xml_diff>
--- a/Weapons Factory - The Project/Reports/Excel/WeaponsFactoryFinancialResult.xlsx
+++ b/Weapons Factory - The Project/Reports/Excel/WeaponsFactoryFinancialResult.xlsx
@@ -5,7 +5,7 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="Rf0fde7b35f0f44ed"/>
+    <sheet name="Sheet1" sheetId="1" r:id="Rce47680ac26f4121"/>
   </sheets>
 </workbook>
 </file>
@@ -183,16 +183,16 @@
         <v>7</v>
       </c>
       <c r="C2" s="0">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" s="0">
         <v>300</v>
       </c>
       <c r="E2" s="0">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0">
-        <v>280</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3">
@@ -203,16 +203,16 @@
         <v>9</v>
       </c>
       <c r="C3" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="0">
         <v>5000</v>
       </c>
       <c r="E3" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="0">
-        <v>4998</v>
+        <v>4999</v>
       </c>
     </row>
     <row r="4">
@@ -223,16 +223,16 @@
         <v>11</v>
       </c>
       <c r="C4" s="0">
-        <v>3686</v>
+        <v>1843</v>
       </c>
       <c r="D4" s="0">
         <v>8800</v>
       </c>
       <c r="E4" s="0">
-        <v>3686</v>
+        <v>1843</v>
       </c>
       <c r="F4" s="0">
-        <v>5114</v>
+        <v>6957</v>
       </c>
     </row>
     <row r="5">
@@ -243,16 +243,16 @@
         <v>11</v>
       </c>
       <c r="C5" s="0">
-        <v>2596</v>
+        <v>1298</v>
       </c>
       <c r="D5" s="0">
         <v>22750</v>
       </c>
       <c r="E5" s="0">
-        <v>2596</v>
+        <v>1298</v>
       </c>
       <c r="F5" s="0">
-        <v>20154</v>
+        <v>21452</v>
       </c>
     </row>
     <row r="6">
@@ -263,16 +263,16 @@
         <v>14</v>
       </c>
       <c r="C6" s="0">
-        <v>2280</v>
+        <v>1140</v>
       </c>
       <c r="D6" s="0">
         <v>23100</v>
       </c>
       <c r="E6" s="0">
-        <v>4560</v>
+        <v>2280</v>
       </c>
       <c r="F6" s="0">
-        <v>18540</v>
+        <v>20820</v>
       </c>
     </row>
     <row r="7">
@@ -283,16 +283,16 @@
         <v>9</v>
       </c>
       <c r="C7" s="0">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="D7" s="0">
         <v>25200</v>
       </c>
       <c r="E7" s="0">
-        <v>168</v>
+        <v>84</v>
       </c>
       <c r="F7" s="0">
-        <v>25032</v>
+        <v>25116</v>
       </c>
     </row>
     <row r="8">
@@ -303,16 +303,16 @@
         <v>17</v>
       </c>
       <c r="C8" s="0">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D8" s="0">
         <v>33000</v>
       </c>
       <c r="E8" s="0">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="F8" s="0">
-        <v>32912</v>
+        <v>32956</v>
       </c>
     </row>
     <row r="9">
@@ -323,16 +323,16 @@
         <v>19</v>
       </c>
       <c r="C9" s="0">
-        <v>4034</v>
+        <v>2017</v>
       </c>
       <c r="D9" s="0">
         <v>64000</v>
       </c>
       <c r="E9" s="0">
-        <v>4034</v>
+        <v>2017</v>
       </c>
       <c r="F9" s="0">
-        <v>59966</v>
+        <v>61983</v>
       </c>
     </row>
     <row r="10">
@@ -343,16 +343,16 @@
         <v>21</v>
       </c>
       <c r="C10" s="0">
-        <v>4216</v>
+        <v>2108</v>
       </c>
       <c r="D10" s="0">
         <v>74800</v>
       </c>
       <c r="E10" s="0">
-        <v>8432</v>
+        <v>4216</v>
       </c>
       <c r="F10" s="0">
-        <v>66368</v>
+        <v>70584</v>
       </c>
     </row>
     <row r="11">
@@ -363,16 +363,16 @@
         <v>23</v>
       </c>
       <c r="C11" s="0">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D11" s="0">
         <v>2000000</v>
       </c>
       <c r="E11" s="0">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F11" s="0">
-        <v>1999800</v>
+        <v>1999900</v>
       </c>
     </row>
     <row r="12">
@@ -383,22 +383,22 @@
         <v>25</v>
       </c>
       <c r="C12" s="0">
-        <v>17152</v>
+        <v>8576</v>
       </c>
       <c r="D12" s="0">
         <v>2256950</v>
       </c>
       <c r="E12" s="0">
-        <v>23786</v>
+        <v>11893</v>
       </c>
       <c r="F12" s="0">
-        <v>2233164</v>
+        <v>2245057</v>
       </c>
     </row>
   </sheetData>
   <headerFooter/>
   <tableParts>
-    <tablePart r:id="R184516d8ee144851"/>
+    <tablePart r:id="R4eba808b704f4d2b"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>